<commit_message>
Revise budget for 0.75 in boards and add cut list.
</commit_message>
<xml_diff>
--- a/Purchasing/Budget.xlsx
+++ b/Purchasing/Budget.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Item</t>
   </si>
@@ -41,21 +41,12 @@
     <t>Total Cost</t>
   </si>
   <si>
-    <t>5/8" baltic birch plywood 30"x30" panel</t>
-  </si>
-  <si>
     <t>panel</t>
   </si>
   <si>
     <t>board foot</t>
   </si>
   <si>
-    <t>European beech 1/2" boards</t>
-  </si>
-  <si>
-    <t>Lumber cut list</t>
-  </si>
-  <si>
     <t>Thickness (in)</t>
   </si>
   <si>
@@ -99,6 +90,18 @@
   </si>
   <si>
     <t>Lumber delivery</t>
+  </si>
+  <si>
+    <t>European beech 3/4" boards</t>
+  </si>
+  <si>
+    <t>3/4" baltic birch plywood 30"x30" panel</t>
+  </si>
+  <si>
+    <t>3/4" natural birch plywood 2'x4' panel</t>
+  </si>
+  <si>
+    <t>Beech cut list</t>
   </si>
 </sst>
 </file>
@@ -106,7 +109,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -147,7 +150,7 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -433,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,7 +453,7 @@
     <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -468,71 +471,70 @@
       </c>
       <c r="F1" s="3"/>
       <c r="H1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1">
         <f>C2*D2</f>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" t="s">
         <v>13</v>
       </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4">
-        <f>ROUNDUP(N21,0)</f>
-        <v>4</v>
       </c>
       <c r="D3" s="1">
         <v>5.5</v>
       </c>
       <c r="E3" s="1">
         <f>C3*D3</f>
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H3">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="I3">
         <v>5</v>
@@ -553,59 +555,77 @@
       </c>
       <c r="N3">
         <f>H3*J3*L3*M3</f>
-        <v>141.73228346456693</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <v>212.5984251968504</v>
+      </c>
+      <c r="O3">
+        <f>SUM(N3:N7)/144</f>
+        <v>5.9465223097112858</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E4" s="1">
         <f>C4*D4</f>
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H4">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J18" si="0">I4+1</f>
+        <f t="shared" ref="J4:J7" si="0">I4+1</f>
         <v>3</v>
       </c>
       <c r="K4">
         <v>600</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L18" si="1">K4/25.4</f>
+        <f t="shared" ref="L4:L7" si="1">K4/25.4</f>
         <v>23.622047244094489</v>
       </c>
       <c r="M4">
         <v>4</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N18" si="2">H4*J4*L4*M4</f>
-        <v>141.73228346456693</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+        <f t="shared" ref="N4:N9" si="2">H4*J4*L4*M4</f>
+        <v>212.5984251968504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>40</v>
+      </c>
+      <c r="E5" s="1">
+        <f>C5*D5</f>
+        <v>40</v>
+      </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -626,24 +646,22 @@
       </c>
       <c r="N5">
         <f t="shared" si="2"/>
-        <v>94.488188976377955</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+        <v>141.73228346456693</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H6">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K6">
         <v>500</v>
@@ -657,17 +675,20 @@
       </c>
       <c r="N6">
         <f t="shared" si="2"/>
-        <v>78.740157480314963</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+        <v>147.63779527559055</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <f>SUM(E2:E5)</f>
+        <v>141</v>
+      </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="I7">
         <v>2</v>
@@ -688,57 +709,57 @@
       </c>
       <c r="N7">
         <f t="shared" si="2"/>
-        <v>94.488188976377955</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+        <v>141.73228346456693</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
     <row r="20" spans="13:14" x14ac:dyDescent="0.3">
       <c r="M20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="N20">
         <f>SUM(N3:N18)</f>
-        <v>551.18110236220468</v>
+        <v>856.29921259842513</v>
       </c>
     </row>
     <row r="21" spans="13:14" x14ac:dyDescent="0.3">
       <c r="M21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="N21">
         <f>N20/144</f>
-        <v>3.8276465441819769</v>
+        <v>5.9465223097112858</v>
       </c>
     </row>
   </sheetData>

</xml_diff>